<commit_message>
rerun to get new name
</commit_message>
<xml_diff>
--- a/combined_excel_output.xlsx
+++ b/combined_excel_output.xlsx
@@ -436,77 +436,77 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>source_file</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Date_of_Issuance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_3</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_4</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Habitat_Type</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Fish_species</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Offset_footprint_size</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Vegetation_Cover</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Boulder</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Woody_coverage</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Instream_structures</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>source_file</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -518,77 +518,77 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>OCR_18-HCAA-00233.json</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>44.1913</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>-78.8722</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>JAN 10 2020</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>The Proponent must install vegetation-enhanced armour stone walls on a 25 m section of the east bank (50 m²) and retrofit 10 parking lot catchbasins with shields along a 565 m section of the Moira River east bank.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Monitoring of offsetting measures for two years post-construction, with annual reports by November 30.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Prohibition on activities adversely impacting offsetting measures and requirement for access permissions.</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Authorization limitations, including compliance with other regulations and prohibition on deleterious substance deposits.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>river bank, parking lot catchbasins</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Channel Darter</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>50 m² vegetation-enhanced armour stone walls, 10 catchbasin shields over 565 m river section</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>80% vegetation survival required for effectiveness</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>armour stone used in revetment</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>None explicitly mentioned</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>catchbasin shields</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>OCR_00233.json</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -596,83 +596,87 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>OCR_14-HCAA-00814.json</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Feb 07/2020</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>The Proponent must implement offsetting measures including marsh habitat creation, tributary restoration, riparian buffer planting, and storm water management pond expansion to mitigate habitat impacts. Contingency measures are required if these measures fail to meet criteria.</t>
+          <t>JUN 05 2015</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Monitoring and reporting are mandatory, including post-construction assessments, fish sampling, and vegetation survival checks. Reports must be submitted by June 14, 2022.</t>
+          <t>development of an operating plan for the Timiskaming Dam to protect fish spawning habitats</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>No deleterious substances may be deposited in water frequented by fish. Work must comply with Fisheries Act and other regulations.</t>
+          <t>monitoring and reporting requirements including annual reports on dam operations, fish recruitment, and contingency measures</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>The Proponent is responsible for all design and safety aspects. Authorization cannot be transferred without prior DFO notification.</t>
+          <t>implementation of adaptive management strategies if deviations from the operating plan impact spawning success</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>marsh habitat, unnamed tributary restoration, riparian buffer, storm water management pond</t>
+          <t>compliance with Species at Risk Act and prohibition on depositing deleterious substances</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>None explicitly listed in section 4; general references to fish utilization in offsetting measures</t>
+          <t>spawning habitats for Lake Sturgeon and Lake Whitefish</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>marsh habitat (expanded sections), Hooper Drain channel (realigned), Lavallee Creek tributary (restored), riparian buffer (80% coverage required), SWM pond (average depth 0.9m)</t>
+          <t>Lake Sturgeon, Lake Whitefish</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>80% survival for aquatic vegetation and riparian plantings</t>
+          <t>None</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Habitat enhancement features (e.g., woody debris) must show no destabilization</t>
+          <t>None</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Habitat enhancement features in channels must remain stable</t>
+          <t>None</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>OCR_00064.json</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>OCR_14-HCAA-00810.json</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>None</t>
@@ -680,47 +684,47 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JUN 05 2015</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>development of an operating plan for the Timiskaming Dam to protect fish spawning habitats</t>
+          <t>may 08 2015</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>monitoring and reporting requirements including annual reports on dam operations, fish recruitment, and contingency measures</t>
+          <t>mitigation measures including fish rescue reporting, habitat offsetting, and compliance with SARA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>implementation of adaptive management strategies if deviations from the operating plan impact spawning success</t>
+          <t>monitoring and reporting requirements for both mitigation and offsetting measures, including annual reports with data and photographs</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>compliance with Species at Risk Act and prohibition on depositing deleterious substances</t>
+          <t>implementation of offsetting measures during construction phase with specific habitat enhancements</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>spawning habitats for Lake Sturgeon and Lake Whitefish</t>
+          <t>prohibition on transferring authorization and requirement to maintain on-site documentation</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Lake Sturgeon, Lake Whitefish</t>
+          <t>river, lake, shoreline, spawning, resting, foraging</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>walleye</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>880 m2 (river habitat from old dam removal), 400 m2 (Walleye spawning and resting), 895 m2 (shoreline/upperland), 720 m2 (lake to river habitat)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -730,7 +734,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>additional boulders for Walleye spawning areas if washed out</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -740,150 +744,146 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>OCR_00814.json</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>rock shoal (5-10m length, 10-40 m2 area)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>53°36'40.96"N</t>
+          <t>OCR_18-HCAA-00064.json</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>108°44'38.01"W</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>FEB 26 2020</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment entering the NSR during all project phases.</t>
+          <t>Feb 07/2020</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fish screens must meet requirements of 0.125 m/s intake flow with 7,045 m² of total screen area to prevent entrainment.</t>
+          <t>The Proponent must implement offsetting measures including marsh habitat creation, tributary restoration, riparian buffer planting, and storm water management pond expansion to mitigate impacts on fish and fish habitat. Contingency measures are required if these measures fail to meet criteria.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Installation of a gravel/cobble bar (5,800 m²) to offset habitat loss, using rounded stone 15–150 mm in diameter.</t>
+          <t>Monitoring and reporting are mandatory, including post-construction assessments, fish sampling, and vegetation survival checks. Reports must be submitted by June 14, 2022.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Monitoring and reporting requirements include post-construction surveys, embeddedness surveys, and functional monitoring over three years.</t>
+          <t>Prohibition on depositing deleterious substances in water frequented by fish. Compliance with other regulatory agencies is required.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>river bank, gravel/cobble bar</t>
+          <t>The Proponent is solely responsible for design and safety of works. Authorization cannot be transferred without prior notification to DFO.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>None explicitly listed in section 4 or elsewhere</t>
+          <t>marsh habitat, unnamed tributary restoration, riparian buffer, storm water management pond, realigned drain channels</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>5800 m2 (gravel/boulder bar)</t>
+          <t>None explicitly listed in section 4; general references to fish utilization and species composition in monitoring sections</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>None specified</t>
+          <t>marsh habitat expansion (size unspecified), unnamed tributary restoration (size unspecified), riparian buffer planting (80% coverage target), Hooper Drain channel (morphology retention), Central Drain channel (morphology retention), SWM pond (average depth 0.9m)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar with stones 15–150 mm</t>
+          <t>80% survival for aquatic vegetation in marsh and 80% coverage for riparian plantings</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>None mentioned</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar installation</t>
+          <t>Habitat enhancement features (e.g., woody debris) in marsh and tributary require no destabilization</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>OCR_00192.json</t>
+          <t>Habitat enhancement features in marsh and tributary must remain stable</t>
         </is>
       </c>
       <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>OCR_18-HCAA-00311.json</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>oct 16, 2019</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>authorization under Fisheries Act for work likely to cause serious harm to fish, requiring compliance with conditions including habitat offsetting, monitoring, and reporting</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>prohibition on depositing deleterious substances in water frequented by fish</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>requirement to obtain access permissions for lands/waters not owned by proponent</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>no transfer of authorization without prior notification to DFO</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>stream, channel, riparian zone, instream habitat features</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>rainbow trout</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>reach sn01, reach sn02, unnamed tributary of seneca creek (specific sizes not quantified in m2)</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>80% survival target for planted vegetation in riparian zone</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>None</t>
@@ -891,12 +891,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
           <t>constructed instream habitat features including channel morphological features, spawning surveys required</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>OCR_00311.json</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -908,77 +908,77 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>OCR_18-HCAA-00192.json</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>53°36'40.96"N</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>may 08 2015</t>
+          <t>108°44'38.01"W</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>mitigation measures including fish rescue reporting, habitat offsetting, and compliance with SARA</t>
+          <t>FEB 26 2020</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>monitoring and reporting requirements for both mitigation and offsetting measures, including annual reports with data and photographs</t>
+          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment entering the NSR during all project phases.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>implementation of offsetting measures to enhance habitats such as walleye spawning areas and rock shoals</t>
+          <t>Fish screens must meet requirements of 0.125 m/s intake flow with 7,045 m² of total screen area to prevent entrainment.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>prohibition on transferring authorization and legal consequences for non-compliance</t>
+          <t>Installation of a gravel/cobble bar (5,800 m²) to offset habitat loss, using rounded stone 15–150 mm in diameter.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>river, lake, shoreline, spawning, resting, foraging</t>
+          <t>Monitoring and reporting requirements include post-construction surveys, embeddedness surveys, and functional monitoring over three years.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>walleye</t>
+          <t>river bank, gravel/cobble bar</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>880 m2 (river habitat from old dam removal), 400 m2 (walleye spawning with rock shoal), 895 m2 (shoreline re-profiling), 720 m2 (lake to river habitat conversion)</t>
+          <t>None explicitly listed in section 4 or elsewhere</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>5800 m2 (gravel/boulder bar)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>installation of boulders as contingency for washed-out spawning areas</t>
+          <t>None specified</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Gravel/boulder bar with stones 15–150 mm</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>rock shoal (5-10m length, 10-40 m2 area)</t>
+          <t>None mentioned</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>OCR_00810.json</t>
+          <t>Gravel/boulder bar installation</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
@@ -986,77 +986,77 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>OCR_18-HCAA-00146.json</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>5672412N</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>11678490E</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>AUG 17 2018</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Sedimentation and erosion control measures must be in place and maintained to avoid sediment release into the watercourse.</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Total suspended sediment and turbidity monitoring must adhere to the plan in Appendix C of the 2018 Aquatic Effects Assessment.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>All riprap must be clean, free of fine materials, and not obtained from fish-frequented waters below the ordinary high water mark.</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Dewatering must direct water to vegetated areas or settling basins, ensuring water quality meets standards before returning to fish habitats.</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>fish habitat (specific type not explicitly stated beyond 'resident fish species' and 'fish-frequented waters')</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>resident fish species (specific species not listed)</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>7,800 m² for the secondary channel regrading downstream</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>None explicitly mentioned beyond general requirements for sediment control and spoil disposal areas</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>Natural structures like large boulders contributing to fish habitat must be stockpiled for replacement post-construction</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>Natural structures including woody debris must be stockpiled for replacement</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Berm construction and riprap placement are noted as in-stream activities with specific mitigation measures</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>OCR_00146.json</t>
         </is>
       </c>
       <c r="P8" t="inlineStr"/>
@@ -1064,77 +1064,77 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>OCR_18-HCAA-00145.json</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>43.79381</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>-80.386060</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>JAN 10 2020</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release during work.</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Fish rescue and relocation required before work in isolated areas.</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Monitoring and reporting including photographic records and as-built surveys.</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Habitat offsetting measures with specific criteria (e.g., overwintering pools, vegetation coverage).</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>fish habitat (permanent alteration, destruction)</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>trout</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>50 m2 (boulder clusters), 100 m2 (sweeper trees), 80% vegetation coverage</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>80%</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>large boulder clusters (50 m2)</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>anchored sweeper trees (100 m2)</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>overwintering pool habitat (1.7m depth), boulder clusters, sweeper trees</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>OCR_00145.json</t>
         </is>
       </c>
       <c r="P9" t="inlineStr"/>
@@ -1142,77 +1142,77 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>OCR_18-HCAA-00253.json</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>50.894225</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>-114.009975</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>feb 04 2018</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release into water. In-water activity timing restrictions to protect spawning fish and their eggs (May 1st to July 15th and September 16th to April 5th).</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Berm construction and removal must adhere to approved plans, with footprint not exceeding 5% of design area without DFO approval. Natural structures must be replaced after construction.</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Revegetation with native plants, equipment cleanliness to prevent invasive species, spill response plans, and stockpiling materials above high water level.</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>3,462 m² of fish habitat restoration upstream/downstream on west bank. Monitoring and reporting on offset effectiveness over three years.</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>river habitat (offsetting measures on west bank)</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>None explicitly listed in the document</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>3462 m²</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>None specified</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>None specified</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>None specified</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>None specified</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>OCR_00253.json</t>
         </is>
       </c>
       <c r="P10" t="inlineStr"/>
@@ -1220,77 +1220,77 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>OCR_18-HCAA-00160.json</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>71.889403°N</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>-80.887592°W</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>March 21, 2019</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>The work must be completed by the expiration date or DFO must be notified for extension.</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Implement sediment and erosion control measures, including approved plans and monitoring turbidity levels.</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Monitor and report on mitigation measures and submit reports by specified dates.</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Offset habitat loss by placing course rock substrate and adhere to contingency plans.</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Intertidal marine habitat, Subtidal marine habitat, Intertidal unnamed stream</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>None explicitly listed in the provided sections</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>2792 HEUs of potential fish habitat</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>None mentioned</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>Course rock substrate placement as part of offset measures</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>None mentioned</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>None mentioned</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>OCR_00160.json</t>
         </is>
       </c>
       <c r="P11" t="inlineStr"/>

</xml_diff>

<commit_message>
added more columns for better analysis
</commit_message>
<xml_diff>
--- a/combined_excel_output.xlsx
+++ b/combined_excel_output.xlsx
@@ -451,67 +451,67 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Coordinates</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Date_of_Issuance</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_3</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Condition_summary_4</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Habitat_Type</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fish_species</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Offset_footprint_size</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Vegetation_Cover</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Boulder</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Woody_coverage</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Instream_structures</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Langitude</t>
         </is>
       </c>
     </row>
@@ -523,62 +523,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>44.1913</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-78.8722</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>JAN 10 2020</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>The Proponent must install vegetation-enhanced armour stone walls on a 25 m section of the east bank (50 m²) and retrofit 10 parking lot catchbasins with shields along a 565 m section of the Moira River east bank.</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Monitoring of offsetting measures for two years post-construction, with annual reports by November 30.</t>
+          <t>Install vegetation-enhanced armour stone walls on a 25 m section of the east bank (50 m²) and retrofit 10 parking lot catchbasins with shields along a 565 m section of the Moira River east bank.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Prohibition on activities adversely impacting offsetting measures and requirement for access permissions.</t>
+          <t>Monitor offsetting measures for two years post-construction, reporting annually by November 30.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Authorization limitations, including compliance with other regulations and prohibition on deleterious substance deposits.</t>
+          <t>Implement contingency measures if offsetting measures fail to meet criteria (e.g., 80% vegetation survival or 50% turbidity reduction).</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>river bank, parking lot catchbasins</t>
+          <t>Prohibit adverse impacts on offsetting measures and ensure DFO access rights for implementation and monitoring.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>Riverine</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>Channel Darter</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>50 m² vegetation-enhanced armour stone walls, 10 catchbasin shields over 565 m river section</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>80% vegetation survival required for effectiveness</t>
+          <t>50 m² vegetation-enhanced stone revetment, 10 catchbasin shields over 565 m river section</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>armour stone used in revetment</t>
+          <t>Riparian vegetation (enhanced through stone revetment)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -588,10 +588,14 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>catchbasin shields</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr"/>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Vegetation-enhanced armour stone walls (structural habitat), catchbasin shields (turbidity reduction infrastructure)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -599,7 +603,11 @@
           <t>OCR_14-HCAA-00814.json</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>None</t>
@@ -607,42 +615,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>JUN 05 2015</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>development of an operating plan for the Timiskaming Dam to protect fish spawning habitats</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>monitoring and reporting requirements including annual reports on dam operations, fish recruitment, and contingency measures</t>
+          <t>Annual dam operation monitoring reports must be submitted by August 31 each year, summarizing dam operations from October 1 to July 15, including deviations from the operating plan and recommendations for changes.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>implementation of adaptive management strategies if deviations from the operating plan impact spawning success</t>
+          <t>Annual reports on juvenile Lake Sturgeon and Lake Whitefish recruitment must be submitted, detailing capture data, locations, substrates, depths, and age assessments using specified methods.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>compliance with Species at Risk Act and prohibition on depositing deleterious substances</t>
+          <t>Contingency monitoring reports for additional offsetting measures must be provided as directed by DFO, describing adaptive management and effectiveness.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>spawning habitats for Lake Sturgeon and Lake Whitefish</t>
+          <t>A final summary report combining all monitoring reports must be submitted within 90 days after the last report.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>Riverine</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>Lake Sturgeon, Lake Whitefish</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>None</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -689,65 +697,69 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>may 08 2015</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>mitigation measures including fish rescue reporting, habitat offsetting, and compliance with SARA</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>monitoring and reporting requirements for both mitigation and offsetting measures, including annual reports with data and photographs</t>
+          <t>offsetting measures must be completed during construction phase and meet criteria in the proponent’s plan</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>implementation of offsetting measures during construction phase with specific habitat enhancements</t>
+          <t>annual monitoring reports required, including fish rescue details and photos</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>prohibition on transferring authorization and requirement to maintain on-site documentation</t>
+          <t>no adverse impact on offsetting measures; compliance with other regulations and sara</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>river, lake, shoreline, spawning, resting, foraging</t>
+          <t>authorization cannot be transferred without dfo notification</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
+          <t>riverine, lake, shoreline</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
           <t>walleye</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>880 m2 (river habitat from old dam removal), 400 m2 (Walleye spawning and resting), 895 m2 (shoreline/upperland), 720 m2 (lake to river habitat)</t>
-        </is>
-      </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>880 m2 (river habitat from old dam removal), 400 m2 (walleye spawning habitat), 895 m2 (shoreside/upperland), 720 m2 (lake to river habitat)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>additional boulders for Walleye spawning areas if washed out</t>
+          <t>None</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>additional boulders to resist displacement if spawning areas wash out (contingency)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>rock shoal (5-10m length, 10-40 m2 area)</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -767,65 +779,69 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Feb 07/2020</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>The Proponent must implement offsetting measures including marsh habitat creation, tributary restoration, riparian buffer planting, and storm water management pond expansion to mitigate impacts on fish and fish habitat. Contingency measures are required if these measures fail to meet criteria.</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Monitoring and reporting are mandatory, including post-construction assessments, fish sampling, and vegetation survival checks. Reports must be submitted by June 14, 2022.</t>
+          <t>The Proponent must conduct monitoring and reporting on offsetting measures, including post-construction assessments and fish sampling, with reports due by June 14, 2022.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Prohibition on depositing deleterious substances in water frequented by fish. Compliance with other regulatory agencies is required.</t>
+          <t>Structural stability and functionality of offsetting habitats must be maintained; contingency measures required if not met.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>The Proponent is solely responsible for design and safety of works. Authorization cannot be transferred without prior notification to DFO.</t>
+          <t>Prohibition on depositing deleterious substances in water frequented by fish.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>marsh habitat, unnamed tributary restoration, riparian buffer, storm water management pond, realigned drain channels</t>
+          <t>Authorization cannot be transferred without prior notification to DFO.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>None explicitly listed in section 4; general references to fish utilization and species composition in monitoring sections</t>
+          <t>Storm water management pond, tributary, drain, marsh</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>marsh habitat expansion (size unspecified), unnamed tributary restoration (size unspecified), riparian buffer planting (80% coverage target), Hooper Drain channel (morphology retention), Central Drain channel (morphology retention), SWM pond (average depth 0.9m)</t>
+          <t>None explicitly listed in the provided sections</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>80% survival for aquatic vegetation in marsh and 80% coverage for riparian plantings</t>
+          <t>Storm water management pond (average depth 0.9m), unnamed tributary restoration, Hooper Drain channel, Central Drain channel, marsh habitat with berm</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>Riparian vegetation (trees and shrubs)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Habitat enhancement features (e.g., woody debris) in marsh and tributary require no destabilization</t>
+          <t>None mentioned</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Habitat enhancement features in marsh and tributary must remain stable</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
+          <t>Habitat enhancement features (e.g., woody debris) in tributary restoration</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Pool/deepwater habitat in SWM pond, riffles in tributary, channel morphology in drains</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -833,7 +849,11 @@
           <t>OCR_18-HCAA-00311.json</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>None</t>
@@ -841,67 +861,67 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>oct 16, 2019</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>authorization under Fisheries Act for work likely to cause serious harm to fish, requiring compliance with conditions including habitat offsetting, monitoring, and reporting</t>
+          <t>Oct 16, 2019</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>prohibition on depositing deleterious substances in water frequented by fish</t>
+          <t>The Proponent must conduct annual monitoring reports on offsetting measures by Dec 31, 2020 and 2021, including photographic records and as-built surveys.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>requirement to obtain access permissions for lands/waters not owned by proponent</t>
+          <t>The Proponent must ensure no adverse impact on offsetting measures and obtain access permissions for DFO to monitor the measures.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>no transfer of authorization without prior notification to DFO</t>
+          <t>The Proponent must implement erosion control measures, prevent deleterious substance deposits, and maintain a spill response plan.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>stream, channel, riparian zone, instream habitat features</t>
+          <t>The Proponent must adhere to the offsetting plan's specifications, including vegetation survival rates and habitat utilization assessments.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>rainbow trout</t>
+          <t>Riverine</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>reach sn01, reach sn02, unnamed tributary of seneca creek (specific sizes not quantified in m2)</t>
+          <t>Rainbow Trout</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>80% survival target for planted vegetation in riparian zone</t>
+          <t>Reach SN01: unspecified; Reach SN02: unspecified; unnamed tributary: unspecified</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Riparian vegetation (e.g., trees, shrubs, and grass)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>constructed instream habitat features including channel morphological features, spawning surveys required</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Pools, riffles, instream habitat features</t>
         </is>
       </c>
     </row>
@@ -923,65 +943,69 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>53°36'40.96"N, 108°44'38.01"W; 12U 58311E E, 5940187 N</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>FEB 26 2020</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment entering the NSR during all project phases.</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Fish screens must meet requirements of 0.125 m/s intake flow with 7,045 m² of total screen area to prevent entrainment.</t>
+          <t>Sediment and erosion control measures including installation of gravel/boulder bar during low flow periods.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Installation of a gravel/cobble bar (5,800 m²) to offset habitat loss, using rounded stone 15–150 mm in diameter.</t>
+          <t>Monitoring of offset structures post-construction for three years, including embeddedness surveys and sonar surveys.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Monitoring and reporting requirements include post-construction surveys, embeddedness surveys, and functional monitoring over three years.</t>
+          <t>Compliance with Species at Risk Act (SARA) restrictions, no harm to listed species or their habitats.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>river bank, gravel/cobble bar</t>
+          <t>Submission of yearly reports (2022-2024) detailing monitoring results and adherence to offset criteria.</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>Riverine</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>None explicitly listed in section 4 or elsewhere</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>5800 m2 (gravel/boulder bar)</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>None specified</t>
+          <t>Gravel/boulder bar installation with area measurement required as per Offsetting Plan</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar with stones 15–150 mm</t>
+          <t>Riparian vegetation (consultation with DFO on specifications)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>None mentioned</t>
+          <t>Gravel/boulder bar installation as part of offset measures</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar installation</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr"/>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Gravel/boulder bar (not extending beyond intake structure)</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1001,65 +1025,69 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>11678490E 5672412N</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>AUG 17 2018</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Sedimentation and erosion control measures must be in place and maintained to avoid sediment release into the watercourse.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Total suspended sediment and turbidity monitoring must adhere to the plan in Appendix C of the 2018 Aquatic Effects Assessment.</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>All riprap must be clean, free of fine materials, and not obtained from fish-frequented waters below the ordinary high water mark.</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Dewatering must direct water to vegetated areas or settling basins, ensuring water quality meets standards before returning to fish habitats.</t>
+          <t>All riprap must be clean and free of fine materials, not obtained from fish-frequented waters.</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>fish habitat (specific type not explicitly stated beyond 'resident fish species' and 'fish-frequented waters')</t>
+          <t>Contingency measures include upgrading erosion controls, increasing berm height, and halting work if turbidity thresholds are met.</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>resident fish species (specific species not listed)</t>
+          <t>Riverine</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>7,800 m² for the secondary channel regrading downstream</t>
+          <t>None explicitly listed in the document</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>None explicitly mentioned beyond general requirements for sediment control and spoil disposal areas</t>
+          <t>7,800 m²</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Natural structures like large boulders contributing to fish habitat must be stockpiled for replacement post-construction</t>
+          <t>Well-vegetated area for dewatering discharge</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Natural structures including woody debris must be stockpiled for replacement</t>
+          <t>Large boulders are to be stockpiled and replaced as part of natural structures preservation.</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Berm construction and riprap placement are noted as in-stream activities with specific mitigation measures</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr"/>
+          <t>Woody debris is to be stockpiled and replaced as part of natural structures preservation.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Secondary channel re-graded to increase connectivity during low flow conditions.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1079,65 +1107,69 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>43.79381, -80.386060</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>JAN 10 2020</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release during work.</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Fish rescue and relocation required before work in isolated areas.</t>
+          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Monitoring and reporting including photographic records and as-built surveys.</t>
+          <t>Qualified environmental professional on-site to monitor instream and shoreline activities.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Habitat offsetting measures with specific criteria (e.g., overwintering pools, vegetation coverage).</t>
+          <t>Fish rescue and relocation in isolated areas before work commences.</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>fish habitat (permanent alteration, destruction)</t>
+          <t>Temporary rock causeways must be installed no sooner than July 1 and removed by September 30 annually.</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
+          <t>Riverine</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
           <t>trout</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>50 m2 (boulder clusters), 100 m2 (sweeper trees), 80% vegetation coverage</t>
-        </is>
-      </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>50 m2 boulder clusters, 100 m2 sweeper trees</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>large boulder clusters (50 m2)</t>
+          <t>Riparian vegetation (e.g. trees and shrubs and grass)</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>anchored sweeper trees (100 m2)</t>
+          <t>Boulder clusters for velocity refuge habitat</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>overwintering pool habitat (1.7m depth), boulder clusters, sweeper trees</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr"/>
+          <t>Anchored sweeper trees</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Overwintering pool habitat with minimum 1.7m depth</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1157,65 +1189,69 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>feb 04 2018</t>
+          <t>Longitude: -114.009975, Latitude: 50.894225</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release into water. In-water activity timing restrictions to protect spawning fish and their eggs (May 1st to July 15th and September 16th to April 5th).</t>
+          <t>FEB 04 2018</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Berm construction and removal must adhere to approved plans, with footprint not exceeding 5% of design area without DFO approval. Natural structures must be replaced after construction.</t>
+          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release into water. Turbidity monitoring follows the 2018 plan. Contingency measures include upgrading erosion controls, adding armor, raising berms, and halting work if thresholds are met.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Revegetation with native plants, equipment cleanliness to prevent invasive species, spill response plans, and stockpiling materials above high water level.</t>
+          <t>3,462 m² of habitat restoration upstream/downstream on the west bank per the offsetting plan. Monitoring reports due by Jan 15, 2023, with three years of post-construction monitoring ending Dec 31, 2025.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>3,462 m² of fish habitat restoration upstream/downstream on west bank. Monitoring and reporting on offset effectiveness over three years.</t>
+          <t>Prohibits deposit of deleterious substances, harming SARA-listed species, or damaging their habitats. Authorization cannot be transferred without DFO approval.</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>river habitat (offsetting measures on west bank)</t>
+          <t>Proponent responsible for all design and safety aspects. Must comply with other regulatory agencies. Reports on mitigation measures post-work with photos and inspection reports.</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
+          <t>Riverine</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
           <t>None explicitly listed in the document</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>3462 m²</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>None specified</t>
-        </is>
-      </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>None specified</t>
+          <t>None explicitly mentioned in offsetting measures</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>None specified</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>None specified</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr"/>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>None explicitly mentioned in offsetting measures</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1235,65 +1271,69 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>71.889403°N, -80.887592°W; Zone: 17 W, Easting: 503900 m E, Northings: 796600 m N</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>March 21, 2019</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>The work must be completed by the expiration date or DFO must be notified for extension.</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Implement sediment and erosion control measures, including approved plans and monitoring turbidity levels.</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Monitor and report on mitigation measures and submit reports by specified dates.</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Offset habitat loss by placing course rock substrate and adhere to contingency plans.</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
+          <t>Offset habitat loss by placing course rock substrate to provide 2792 HEUs of habitat and implement contingency plans if needed.</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>Intertidal marine habitat, Subtidal marine habitat, Intertidal unnamed stream</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>None explicitly listed in the provided sections</t>
-        </is>
-      </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>None explicitly mentioned in the document</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>2792 HEUs of potential fish habitat</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>None mentioned</t>
-        </is>
-      </c>
       <c r="M11" t="inlineStr">
         <is>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
           <t>Course rock substrate placement as part of offset measures</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>None mentioned</t>
-        </is>
-      </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>None mentioned</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr"/>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>None explicitly mentioned</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new file, run the old way
</commit_message>
<xml_diff>
--- a/combined_excel_output.xlsx
+++ b/combined_excel_output.xlsx
@@ -523,17 +523,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>43.9583</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>-80.0473</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>43.9583, -80.0473</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -543,22 +543,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Install vegetation-enhanced armour stone walls on a 25 m section of the east bank (50 m²) and retrofit 10 parking lot catchbasins with shields along a 565 m section of the Moira River east bank.</t>
+          <t>The Proponent must implement vegetation-enhanced stone revetment and catchbasin shields as offsetting measures by September 30, 2021, with monitoring for vegetation survival (80%) and turbidity reduction (50%).</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Monitor offsetting measures for two years post-construction, reporting annually by November 30.</t>
+          <t>The Proponent must not carry out any activities that adversely impact the offsetting measures and must provide access permissions for DFO to monitor them.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Implement contingency measures if offsetting measures fail to meet criteria (e.g., 80% vegetation survival or 50% turbidity reduction).</t>
+          <t>The authorization may be revoked or amended if necessary to protect species at risk, and compliance is mandatory to avoid legal consequences.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Prohibit adverse impacts on offsetting measures and ensure DFO access rights for implementation and monitoring.</t>
+          <t>The Proponent must submit annual monitoring reports for two years post-construction and ensure all offset measures meet effectiveness criteria.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -571,29 +571,27 @@
           <t>Channel Darter</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>50 m² vegetation-enhanced stone revetment, 10 catchbasin shields over 565 m river section</t>
-        </is>
+      <c r="L2" t="n">
+        <v>100</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Riparian vegetation (enhanced through stone revetment)</t>
+          <t>Riparian vegetation (e.g. trees and shrubs and grass)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Vegetation-enhanced armour stone walls (structural habitat), catchbasin shields (turbidity reduction infrastructure)</t>
+          <t>Riffles (rivers)</t>
         </is>
       </c>
     </row>
@@ -625,22 +623,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Annual dam operation monitoring reports must be submitted by August 31 each year, summarizing dam operations from October 1 to July 15, including deviations from the operating plan and recommendations for changes.</t>
+          <t>The Proponent must implement offsetting measures to address serious harm to fish, including habitat restoration and creation as per the operating plan.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Annual reports on juvenile Lake Sturgeon and Lake Whitefish recruitment must be submitted, detailing capture data, locations, substrates, depths, and age assessments using specified methods.</t>
+          <t>Annual monitoring reports required for dam operations, fish species, and contingency measures, with specific submission deadlines and data formats.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Contingency monitoring reports for additional offsetting measures must be provided as directed by DFO, describing adaptive management and effectiveness.</t>
+          <t>Prohibition on depositing deleterious substances and compliance with Species at Risk Act requirements.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>A final summary report combining all monitoring reports must be submitted within 90 days after the last report.</t>
+          <t>Authorization cannot be transferred without prior notification to DFO, and non-compliance may result in legal action.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -675,7 +673,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Riffles (rivers)</t>
         </is>
       </c>
     </row>
@@ -702,43 +700,41 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>may 08 2015</t>
+          <t>MAY 08 2015</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>offsetting measures must be completed during construction phase and meet criteria in the proponent’s plan</t>
+          <t>The Proponent must complete offsetting measures during construction phase, including habitat enhancements and rock shoal installation.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>annual monitoring reports required, including fish rescue details and photos</t>
+          <t>Monitoring and reporting requirements include annual reports by March 1st, detailing fish rescue efforts, habitat effectiveness, and any adaptive measures.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>no adverse impact on offsetting measures; compliance with other regulations and sara</t>
+          <t>No adverse impacts on offsetting measures are allowed, and compliance with other regulations (e.g., SARA) is mandatory.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>authorization cannot be transferred without dfo notification</t>
+          <t>Authorization cannot be transferred without prior notification to DFO, and all work must adhere to design and safety standards.</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>riverine, lake, shoreline</t>
+          <t>Riverine</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>walleye</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>880 m2 (river habitat from old dam removal), 400 m2 (walleye spawning habitat), 895 m2 (shoreside/upperland), 720 m2 (lake to river habitat)</t>
-        </is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>2095</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -747,7 +743,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>additional boulders to resist displacement if spawning areas wash out (contingency)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -757,7 +753,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>rock shoal (5-10m length, 10-40 m2 area)</t>
+          <t>Rock shoal, shoreline re-profiling for spawning, and lake-to-river habitat conversion</t>
         </is>
       </c>
     </row>
@@ -789,42 +785,40 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>The Proponent must conduct monitoring and reporting on offsetting measures, including post-construction assessments and fish sampling, with reports due by June 14, 2022.</t>
+          <t>The Proponent must conduct post-construction monitoring and submit a report by June 14, 2022, ensuring offsetting measures meet criteria.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Structural stability and functionality of offsetting habitats must be maintained; contingency measures required if not met.</t>
+          <t>Structural stability and functionality of offsetting habitat must be maintained; contingency measures required if not met.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Prohibition on depositing deleterious substances in water frequented by fish.</t>
+          <t>Prohibition on adverse disturbance of offsetting measures without DFO approval.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Authorization cannot be transferred without prior notification to DFO.</t>
+          <t>Proponent must inform DFO of any unauthorized impacts to fish or habitat and comply with all conditions to avoid legal penalties.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Storm water management pond, tributary, drain, marsh</t>
+          <t>Riverine, Estuarine, Lentic</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>None explicitly listed in the provided sections</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Storm water management pond (average depth 0.9m), unnamed tributary restoration, Hooper Drain channel, Central Drain channel, marsh habitat with berm</t>
-        </is>
+          <t>None explicitly listed in section 4</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>1000</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Riparian vegetation (trees and shrubs)</t>
+          <t>Riparian vegetation (e.g. trees and shrubs and grass)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -834,12 +828,12 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Habitat enhancement features (e.g., woody debris) in tributary restoration</t>
+          <t>Habitat enhancement features including woody debris or structures</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Pool/deepwater habitat in SWM pond, riffles in tributary, channel morphology in drains</t>
+          <t>Pool/deepwater habitat, riffles, mesostructural units</t>
         </is>
       </c>
     </row>
@@ -871,22 +865,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>The Proponent must conduct annual monitoring reports on offsetting measures by Dec 31, 2020 and 2021, including photographic records and as-built surveys.</t>
+          <t>serious harm to fish as described in the authorization</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>The Proponent must ensure no adverse impact on offsetting measures and obtain access permissions for DFO to monitor the measures.</t>
+          <t>compliance with reporting requirements including annual reports by December 31 each year</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>The Proponent must implement erosion control measures, prevent deleterious substance deposits, and maintain a spill response plan.</t>
+          <t>implementation of offsetting measures as per the approved plan</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>The Proponent must adhere to the offsetting plan's specifications, including vegetation survival rates and habitat utilization assessments.</t>
+          <t>provision of access permissions for DFO to monitor offsetting measures</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -901,27 +895,27 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Reach SN01: unspecified; Reach SN02: unspecified; unnamed tributary: unspecified</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Riparian vegetation (e.g., trees, shrubs, and grass)</t>
+          <t>Riparian vegetation (e.g. trees and shrubs and grass)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Pools, riffles, instream habitat features</t>
+          <t>Pool/deepwater habitat, Riffles (rivers)</t>
         </is>
       </c>
     </row>
@@ -943,7 +937,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>53°36'40.96"N, 108°44'38.01"W; 12U 58311E E, 5940187 N</t>
+          <t>53°36'40.96"N, 108°44'38.01"W, UTM Coordinates: [Not explicitly converted, but mentioned in the document]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -953,22 +947,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sediment and erosion control measures including installation of gravel/boulder bar during low flow periods.</t>
+          <t>Installation of gravel/boulder bar during low flow period (fall), not extending further than the river water intake structure</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Monitoring of offset structures post-construction for three years, including embeddedness surveys and sonar surveys.</t>
+          <t>Monitoring of offset structure post-construction for three years including sonar surveys and embeddedness surveys</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Compliance with Species at Risk Act (SARA) restrictions, no harm to listed species or their habitats.</t>
+          <t>Compliance reports due annually by March 31 from 2022 to 2024</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Submission of yearly reports (2022-2024) detailing monitoring results and adherence to offset criteria.</t>
+          <t>Proponent responsible for design and workmanship; authorization non-transferable</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -983,27 +977,27 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar installation with area measurement required as per Offsetting Plan</t>
+          <t>The gravel/boulder bar offset area is specified as requiring a measured area per the Offsetting Plan, but the exact numerical value isn't explicitly stated in the provided text. However, the embeddedness survey and monitoring parameters suggest an area, but without a specific number given.</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Riparian vegetation (consultation with DFO on specifications)</t>
+          <t>None explicitly mentioned in the context of vegetation cover types like emergent or riparian</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar installation as part of offset measures</t>
+          <t>Gravel/boulder bar installation as part of offsetting measures</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None mentioned</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Gravel/boulder bar (not extending beyond intake structure)</t>
+          <t>Gravel/boulder bar (as a structure), riffles implied through velocity distribution monitoring</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1029,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Sedimentation and erosion control measures must be in place and maintained to avoid sediment release into the watercourse.</t>
+          <t>Sedimentation and erosion control measures must be in place and upgraded/maintained to avoid sediment release into the water.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1045,12 +1039,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>All riprap must be clean and free of fine materials, not obtained from fish-frequented waters.</t>
+          <t>All riprap must be clean, free of fine materials, and not obtained from fish-frequented waters below the ordinary high water mark.</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Contingency measures include upgrading erosion controls, increasing berm height, and halting work if turbidity thresholds are met.</t>
+          <t>Water from dewatering must be released into vegetated areas or settling basins and not directly into fish-frequented waters.</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1060,32 +1054,32 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>None explicitly listed in the document</t>
+          <t>None explicitly listed in the provided sections</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>7,800 m²</t>
+          <t>7800 m2</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Well-vegetated area for dewatering discharge</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Large boulders are to be stockpiled and replaced as part of natural structures preservation.</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Woody debris is to be stockpiled and replaced as part of natural structures preservation.</t>
+          <t>None explicitly mentioned</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Secondary channel re-graded to increase connectivity during low flow conditions.</t>
+          <t>Secondary channel re-graded to increase connectivity during low flow conditions</t>
         </is>
       </c>
     </row>
@@ -1117,22 +1111,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release.</t>
+          <t>Inspection reports with dated and annotated photographs during pre-construction, construction, and post-construction periods.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Qualified environmental professional on-site to monitor instream and shoreline activities.</t>
+          <t>Monitoring as per the proposed plan 'Ministry of Transportation – West Region, Highway 401 Grand River Bridge Replacements, Ministry Act Authorization Permit Application Package'.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Fish rescue and relocation in isolated areas before work commences.</t>
+          <t>Contingency measures to prevent greater impacts if mitigation measures fail.</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Temporary rock causeways must be installed no sooner than July 1 and removed by September 30 annually.</t>
+          <t>Completion of offsetting measures by December 31, 2024, with as-built surveys and photographic documentation.</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1147,27 +1141,27 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>50 m2 boulder clusters, 100 m2 sweeper trees</t>
+          <t>150 m2</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Riparian vegetation (e.g. trees and shrubs and grass)</t>
+          <t>80% coverage of herbaceous ground cover and seasonal planted stock</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Boulder clusters for velocity refuge habitat</t>
+          <t>50 m2</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Anchored sweeper trees</t>
+          <t>100 m2</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Overwintering pool habitat with minimum 1.7m depth</t>
+          <t>overwintering pool habitat with depths ≥1.7m, boulder clusters as velocity refuge, anchored sweeper trees</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1183,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Longitude: -114.009975, Latitude: 50.894225</t>
+          <t>Longitude and latitude: 50.894225, -114.009975</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1199,27 +1193,27 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sediment and erosion control measures must be in place and maintained to avoid sediment release into water. Turbidity monitoring follows the 2018 plan. Contingency measures include upgrading erosion controls, adding armor, raising berms, and halting work if thresholds are met.</t>
+          <t>measures and standards to avoid and mitigate serious harm to fish shall be implemented before, during, and following in-water work</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3,462 m² of habitat restoration upstream/downstream on the west bank per the offsetting plan. Monitoring reports due by Jan 15, 2023, with three years of post-construction monitoring ending Dec 31, 2025.</t>
+          <t>monitoring and reporting of implementation of offsetting measures with post-construction monitoring for three years</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Prohibits deposit of deleterious substances, harming SARA-listed species, or damaging their habitats. Authorization cannot be transferred without DFO approval.</t>
+          <t>offsetting measures (3,462 m2) to be completed upstream and downstream on the west bank according to the approved plan</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Proponent responsible for all design and safety aspects. Must comply with other regulatory agencies. Reports on mitigation measures post-work with photos and inspection reports.</t>
+          <t>contingency measures must be reviewed and approved by DFO if mitigation measures fail or offsetting measures are not effective</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Riverine</t>
+          <t>riverine</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1229,12 +1223,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>3462 m²</t>
+          <t>3462 m2</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>None explicitly mentioned in offsetting measures</t>
+          <t>None explicitly mentioned in the offsetting measures</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1249,7 +1243,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>None explicitly mentioned in offsetting measures</t>
+          <t>None explicitly mentioned in the offsetting measures</t>
         </is>
       </c>
     </row>
@@ -1286,17 +1280,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Implement sediment and erosion control measures, including approved plans and monitoring turbidity levels.</t>
+          <t>Sediment and erosion control measures must be implemented and monitored, including approved plans and turbidity monitoring.</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Monitor and report on mitigation measures and submit reports by specified dates.</t>
+          <t>Offsetting measures include placing course rock substrate to provide 2792 HEUs of habitat.</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Offset habitat loss by placing course rock substrate to provide 2792 HEUs of habitat and implement contingency plans if needed.</t>
+          <t>Monitoring and reporting requirements for offsetting measures over ten years, including photographic records and annual reports.</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1306,32 +1300,32 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>None explicitly mentioned in the document</t>
+          <t>None</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2792 HEUs of potential fish habitat</t>
+          <t>2792</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Course rock substrate placement as part of offset measures</t>
+          <t>None</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>None explicitly mentioned</t>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>